<commit_message>
MOD: adding xlsx files
</commit_message>
<xml_diff>
--- a/factura.xlsx
+++ b/factura.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>FacturaID</t>
   </si>
@@ -34,19 +34,22 @@
     <t>MedioPago</t>
   </si>
   <si>
-    <t>00100001010000318051</t>
-  </si>
-  <si>
-    <t>2024-08-08T19:42:12</t>
-  </si>
-  <si>
-    <t>3101109180</t>
-  </si>
-  <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>1</t>
+    <t>00100004010000032593</t>
+  </si>
+  <si>
+    <t>2024-08-09T07:20:26</t>
+  </si>
+  <si>
+    <t>3101775072</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>Credito 17</t>
+  </si>
+  <si>
+    <t>03</t>
   </si>
 </sst>
 </file>
@@ -447,7 +450,7 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Distleimi:Base de datos respaldada exitosamente
</commit_message>
<xml_diff>
--- a/factura.xlsx
+++ b/factura.xlsx
@@ -34,22 +34,22 @@
     <t>MedioPago</t>
   </si>
   <si>
-    <t>00100001010002038940</t>
-  </si>
-  <si>
-    <t>2025-02-21T01:28:34-06:00</t>
-  </si>
-  <si>
-    <t>3101172267</t>
-  </si>
-  <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>99</t>
+    <t>00100102010000009206</t>
+  </si>
+  <si>
+    <t>2025-03-31T10:24:00-06:00</t>
+  </si>
+  <si>
+    <t>3101135332</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>04</t>
   </si>
 </sst>
 </file>

</xml_diff>